<commit_message>
Updated ITA model - 2025-08-15 16:14
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/Sets-vervestacks.xlsx
+++ b/VerveStacks_ITA/Sets-vervestacks.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr updateLinks="never" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VerveStacks\assumptions\VerveStacks_ISO_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA_grids\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10405469-30EC-4378-ACAC-536A51F17F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="1"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="VEDA_Sets-Comm" sheetId="2" r:id="rId3"/>
-    <sheet name="VEDA_Sets-Proc" sheetId="1" r:id="rId4"/>
+    <sheet name="VEDA_Sets-Comm" sheetId="2" r:id="rId1"/>
+    <sheet name="VEDA_Sets-Proc" sheetId="1" r:id="rId2"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="61">
   <si>
     <t>~TFM_Psets</t>
   </si>
@@ -211,25 +211,28 @@
   </si>
   <si>
     <t>-*SMR</t>
+  </si>
+  <si>
+    <t>Grid</t>
+  </si>
+  <si>
+    <t>IRE</t>
+  </si>
+  <si>
+    <t>g[_]*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -269,130 +272,38 @@
       <right/>
       <top/>
       <bottom style="thick">
-        <color theme="4" tint="0.499980002641678"/>
+        <color theme="4" tint="0.49995422223578601"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.399980008602142"/>
+        <color theme="4" tint="0.39997558519241921"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="20"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="21"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="3">
+    <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="2" builtinId="18"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="15" builtinId="5"/>
-    <cellStyle name="Currency" xfId="16" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
-    <cellStyle name="Comma" xfId="18" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
-    <cellStyle name="Heading 2" xfId="20" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="21" builtinId="18"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -700,29 +611,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB068F12-506D-4B74-BF24-03EBDA23C84D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB068F12-506D-4B74-BF24-03EBDA23C84D}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="A3" sqref="A3:H9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="65.8571428571429" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.86328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="56" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.8571428571429" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.4285714285714" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.71428571428571" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="14.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -754,30 +663,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71754C8A-E599-4286-919F-11B5789CC171}">
-  <dimension ref="A1:J20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71754C8A-E599-4286-919F-11B5789CC171}">
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="86" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.4285714285714" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5714285714286" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.8571428571429" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.4285714285714" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="17.25" thickBot="1">
+    <row r="1" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" thickTop="1" thickBot="1">
+    <row r="2" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -809,7 +717,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="14.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>38</v>
       </c>
@@ -826,7 +734,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="14.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>25</v>
       </c>
@@ -834,7 +742,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="14.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>26</v>
       </c>
@@ -842,7 +750,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="14.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>27</v>
       </c>
@@ -850,7 +758,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="14.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>39</v>
       </c>
@@ -864,7 +772,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="14.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>40</v>
       </c>
@@ -872,7 +780,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="14.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>42</v>
       </c>
@@ -880,7 +788,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="14.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>41</v>
       </c>
@@ -888,7 +796,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="14.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>37</v>
       </c>
@@ -896,7 +804,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="4:6" ht="14.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="D12" t="s">
         <v>50</v>
       </c>
@@ -904,7 +812,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="14.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B13" s="3" t="s">
         <v>30</v>
       </c>
@@ -915,7 +823,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="14.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
         <v>31</v>
       </c>
@@ -926,7 +834,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="4:6" ht="14.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="D15" t="s">
         <v>52</v>
       </c>
@@ -934,7 +842,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="14.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -945,7 +853,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="14.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B17" t="s">
         <v>57</v>
       </c>
@@ -962,7 +870,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="14.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -973,7 +881,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="14.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -990,7 +898,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="14.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -999,6 +907,17 @@
       </c>
       <c r="F20" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated ITA model - 2025-09-01 09:24
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/Sets-vervestacks.xlsx
+++ b/VerveStacks_ITA/Sets-vervestacks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr updateLinks="never" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VerveStacks\assumptions\VerveStacks_ISO_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45088BA-E355-4D59-B6D8-AA94E14D9181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A38655E-6B1F-4782-84B6-410D76B8449D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="96">
   <si>
     <t>~TFM_Psets</t>
   </si>
@@ -117,12 +117,6 @@
     <t>Wind offshore</t>
   </si>
   <si>
-    <t>-*WOF*</t>
-  </si>
-  <si>
-    <t>*WOF*</t>
-  </si>
-  <si>
     <t>STG</t>
   </si>
   <si>
@@ -174,9 +168,6 @@
     <t>solar</t>
   </si>
   <si>
-    <t>wind</t>
-  </si>
-  <si>
     <t>geothermal</t>
   </si>
   <si>
@@ -328,6 +319,12 @@
   </si>
   <si>
     <t>Transformers Dn</t>
+  </si>
+  <si>
+    <t>windon</t>
+  </si>
+  <si>
+    <t>windoff</t>
   </si>
 </sst>
 </file>
@@ -1045,39 +1042,39 @@
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D24" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D25" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B27" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D27" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D28" t="str">
         <f>B28</f>
@@ -1086,7 +1083,7 @@
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D29" t="str">
         <f>B29</f>
@@ -1095,7 +1092,7 @@
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B30" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D30" t="str">
         <f>B30</f>
@@ -1104,7 +1101,7 @@
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D31" t="str">
         <f>B31</f>
@@ -1113,39 +1110,39 @@
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B32" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D32" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B33" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D33" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B34" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D34" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B35" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D35" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B36" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D36" t="str">
         <f>B36</f>
@@ -1154,7 +1151,7 @@
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B37" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D37" t="str">
         <f>B37</f>
@@ -1175,7 +1172,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1226,7 +1223,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F3" t="s">
         <v>18</v>
@@ -1235,10 +1232,10 @@
         <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
@@ -1246,7 +1243,7 @@
         <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
@@ -1254,26 +1251,26 @@
         <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F6" t="s">
         <v>19</v>
       </c>
       <c r="H6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F7" t="s">
         <v>20</v>
@@ -1281,7 +1278,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F8" t="s">
         <v>21</v>
@@ -1289,45 +1286,40 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="D11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F11" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B12" s="3" t="s">
-        <v>26</v>
-      </c>
+      <c r="B12" s="3"/>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="F12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>95</v>
       </c>
       <c r="F13" t="s">
         <v>25</v>
@@ -1335,10 +1327,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="D14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F14" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.45">
@@ -1346,13 +1338,13 @@
         <v>11</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F15" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.45">
@@ -1360,121 +1352,121 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D16" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B17" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H17" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I17" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D18" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F18" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" t="s">
         <v>28</v>
-      </c>
-      <c r="B19" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H20" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I20" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F22" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F23" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B24" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F24" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B25" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F25" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.45">
@@ -1752,18 +1744,18 @@
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B47" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F47" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B48" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F48" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>